<commit_message>
Automation test added for QA-569
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile_Ph2.xlsx
+++ b/binaries/FCfiles/FCFile_Ph2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="73">
   <si>
     <t>shipmentType</t>
   </si>
@@ -367,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -390,6 +390,9 @@
     <xf applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="6" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -826,7 +829,7 @@
       <c r="H2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="52" t="s">
+      <c r="Q2" s="68" t="s">
         <v>60</v>
       </c>
     </row>
@@ -873,7 +876,7 @@
       <c r="P3" s="6">
         <v>1</v>
       </c>
-      <c r="Q3" s="55" t="s">
+      <c r="Q3" s="69" t="s">
         <v>60</v>
       </c>
     </row>
@@ -923,7 +926,7 @@
       <c r="P4" s="6">
         <v>1</v>
       </c>
-      <c r="Q4" s="58" t="s">
+      <c r="Q4" s="70" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>